<commit_message>
change number color when less than 80
</commit_message>
<xml_diff>
--- a/public/test22.xlsx
+++ b/public/test22.xlsx
@@ -21,9 +21,6 @@
     <t>Agent</t>
   </si>
   <si>
-    <t>Surveys</t>
-  </si>
-  <si>
     <t>KCSAT</t>
   </si>
   <si>
@@ -58,6 +55,9 @@
   </si>
   <si>
     <t>tasnem.elbasha@tabby.ai</t>
+  </si>
+  <si>
+    <t>Surveyss</t>
   </si>
 </sst>
 </file>
@@ -493,7 +493,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -509,18 +509,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="4">
         <v>170</v>
@@ -534,7 +534,7 @@
     </row>
     <row r="3" spans="1:4" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="4">
         <v>97</v>
@@ -548,7 +548,7 @@
     </row>
     <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="4">
         <v>118</v>
@@ -562,7 +562,7 @@
     </row>
     <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="4">
         <v>91</v>
@@ -576,7 +576,7 @@
     </row>
     <row r="6" spans="1:4" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="4">
         <v>82</v>
@@ -590,7 +590,7 @@
     </row>
     <row r="7" spans="1:4" ht="54" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="4">
         <v>124</v>
@@ -604,7 +604,7 @@
     </row>
     <row r="8" spans="1:4" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="4">
         <v>164</v>
@@ -618,7 +618,7 @@
     </row>
     <row r="9" spans="1:4" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="4">
         <v>169</v>
@@ -630,9 +630,9 @@
         <v>0.76280000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="4">
         <v>108</v>
@@ -644,9 +644,9 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="4">
         <v>96</v>

</xml_diff>